<commit_message>
Comments on the 'supervisor preference versus supervisor no-preference' problem in test spreadsheet 6
</commit_message>
<xml_diff>
--- a/pdn_project_allocation/testdata/test6_multiple_students_per_project.xlsx
+++ b/pdn_project_allocation/testdata/test6_multiple_students_per_project.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Student_preferences" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Supervisor_preferences" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="COMMENTS" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
   <si>
     <t xml:space="preserve">Project_name</t>
   </si>
@@ -94,6 +95,60 @@
   </si>
   <si>
     <t xml:space="preserve">S10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try this one with different supervisor weights.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With supervisor weight 0, students S1 and S2 get their preference of project P1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">But with supervisors weights e.g. 0.25-5, they get pulled towards project P2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">… because supervisor P2, who cares, is giving them supervisor dissatisfaction scores of 1 and 2...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">… and supervisor P1, who doesn’t care, is by default giving all students scores of 5.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">… so the supervisors are “happier” if both students are allocated to P2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(And with weight 0.2, student S2 gets pulled to project P2 but student S1 stays with project P1.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is all logically consistent.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It’s not clear there’s a better method:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- if supervisors who don't get a preference allocate 0 for each student (not 5.5), that pulls students towards them, rather than away</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- if we allocated them the mean expressed preference for supervisors who expressed a preference, that cannot be done (or is not consistent) when some supervisors rank 2 students, some rank 4, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The only question is how much the supervisors should be allowed to influence things (definitely not zero; as a matter of policy less than student preferences).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The other question is whether this causes any problems in practice.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(NB A previous computer-based attempt in PDF failed, i.e. caused unhappiness and needed redoing manually, but we have reason to believe it wasn’t very sophisticated computationally, using ?LiveCode.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://en.wikipedia.org/wiki/LiveCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://livecode.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">… which, while not entirely incapable, does not look like it has an integer programming library, and I would not want to create one for scratch for it as it looks dreadful.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">… Google: “livecode” “integer programming” – 0 hits</t>
   </si>
 </sst>
 </file>
@@ -192,7 +247,7 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -316,7 +371,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -524,7 +579,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -621,6 +676,123 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>